<commit_message>
TAble abbreviations and validation sources added
</commit_message>
<xml_diff>
--- a/Table Additions/Table1_with_uncertainties-From Messina.xlsx
+++ b/Table Additions/Table1_with_uncertainties-From Messina.xlsx
@@ -23,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alex Messina</author>
+  </authors>
+  <commentList>
+    <comment ref="H18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alex Messina:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Venturini 2004 cited in text but not found in References</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t xml:space="preserve">Advantages </t>
   </si>
@@ -535,14 +569,6 @@
     <t xml:space="preserve">    Overall</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean error 0.12 and  5% compared with ETf and annual ET from flux towers and soil moisture balance, respectively (Nagler et al., 2013)
-RSMD 10-30% compared to mean ET from ????? (Glenn et al., 2010); 
-Mean error 4% compared with daily ET from eddy covariance towers (Samani et al., 2009); 
-Mean error 15% compared with daily ET from ground measurements ?? (Duchemin et al., 2006); 
-RMSE 15% compared with daily ET from measured water use ?? (Hunsaker et al., 2007a, 2007b);  
-</t>
-  </si>
-  <si>
     <t>Mean error 13%  compared with of mean annual ET from eddy covariance towers (Fisher et al, 2008)</t>
   </si>
   <si>
@@ -593,8 +619,16 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Mean error 0.12 and  5% compared with ETf and annual ET from flux towers and soil moisture balance, respectively (Nagler et al., 2013)
+RSMD 10-30% compared to seasonal ET from flux towers and water balance(Glenn et al., 2010); 
+Mean error 4% compared with daily ET from eddy covariance towers (Samani et al., 2009); 
+Mean error 15% compared with daily ET from ground radiometers and eddy covariance towers (Duchemin et al., 2006); 
+RMSE 15% compared with daily ET from soil water measurements (Hunsaker et al., 2007a, 2007b);  
+</t>
+  </si>
+  <si>
     <t>RMSE 15-20% compared to daily ET from eddy covariance towers (Allen et al., 2011);
-RMSE ~5% compared to seasonal ET estimates (Bastiaanssen et al., 2005)</t>
+RMSE 1-5% compared to seasonal ET, ~4% for annual estimates from catchment water balances (Bastiaanssen et al., 2005)</t>
   </si>
   <si>
     <r>
@@ -655,7 +689,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> 0.77 compared to λET from ??? (Anderson et al., 1997)
+      <t xml:space="preserve"> 0.77 compared to λET from FIFE,Monsoon '90 (Anderson et al., 1997)
 RMSD 40-50 W m</t>
     </r>
     <r>
@@ -675,20 +709,16 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">  compared to ??? (Norman et al., 2003);
-MAD 15-20% for 30min avg, 10% daily, and ~5% seasonal, compared to ??? (Anderson et al., 2013)</t>
-    </r>
-  </si>
-  <si>
-    <t>Mean error &lt; 30% compared to ??? (Senay et al., 2007); 
-Mean error ~60% on regional or national scale compared to ??? (Velpuri et al., 2013)</t>
-  </si>
-  <si>
-    <t>Mean error 15-40% compared to??? (Allen et al., 2011)</t>
-  </si>
-  <si>
-    <r>
-      <t>RSMD ~30% compared to mean ET from ??? (Jiang and Islam, 2001); 
+      <t xml:space="preserve">  compared to Southern Great Plains flux towers (Norman et al., 2003);
+MAD 15-20% for 30min avg, 10% daily, and ~5% seasonal, compared to AmeriFlux stations Anderson et al., 2013)</t>
+    </r>
+  </si>
+  <si>
+    <t>Mean error ~60% on regional or national scale compared to annual ET from FLUXNET and water balance(Velpuri et al., 2013)</t>
+  </si>
+  <si>
+    <r>
+      <t>RSMD ~30% compared to mean ET from eddy covariance and Bowen Ratio observations (Jiang and Islam, 2001); 
 RMSD 45 Wm</t>
     </r>
     <r>
@@ -770,7 +800,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>compared to instantaneous λET from??  (Moran 1996); 
+      <t>compared to instantaneous λET from a MetFlux station  (Moran 1996); 
 RMSD 59 Wm</t>
     </r>
     <r>
@@ -882,7 +912,34 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>compared to daily ET  in situ ?? (Z</t>
+      <t xml:space="preserve">compared to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.199999999999999"/>
+        <color theme="1"/>
+        <rFont val="Cambria Math"/>
+        <family val="1"/>
+      </rPr>
+      <t>λ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.65"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ET </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.199999999999999"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>from Bowen Ratio (Z</t>
     </r>
     <r>
       <rPr>
@@ -892,7 +949,7 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">ahira et al. (2009); 
-RMSE 25–32%  compared to mean daily ET from ???? (Bhattacharya et al., 2010); </t>
+RMSE 25–32%  compared to λET from in situ energy balance measurements (Bhattacharya et al., 2010); </t>
     </r>
   </si>
   <si>
@@ -917,13 +974,13 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> 0.61 compared to Λ  from ??? (Wang et al 2006)</t>
+      <t xml:space="preserve"> 0.61 compared to Λ  from Bowen Ratio (Wang et al 2006)</t>
     </r>
   </si>
   <si>
     <r>
       <t>RMSD ±10% for daily ET from FIFE/MONSOON (Gillies et al., 1997);
-Error ~ 15-50% for λET from in situ and airborne ??? (Brunsell and Gillies, 2003); 
+Error ~ 15-50% for λET from eddy covariance stations at SGP97 (Brunsell and Gillies, 2003); 
 RMSD 7 Wm</t>
     </r>
     <r>
@@ -952,7 +1009,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,6 +1070,31 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10.199999999999999"/>
+      <color theme="1"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8.65"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1107,26 +1189,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1407,11 +1489,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
@@ -1426,26 +1508,26 @@
     <col min="5" max="5" width="29.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="29.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="88.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="97.7109375" style="10" customWidth="1"/>
     <col min="9" max="9" width="42.140625" style="12" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="2:9" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="14" t="s">
         <v>0</v>
       </c>
@@ -1477,10 +1559,10 @@
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
@@ -1494,17 +1576,17 @@
         <v>29</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="7" t="s">
         <v>35</v>
       </c>
@@ -1518,17 +1600,17 @@
         <v>28</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1542,34 +1624,34 @@
         <v>7</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>81</v>
@@ -1585,10 +1667,10 @@
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="7" t="s">
         <v>38</v>
       </c>
@@ -1608,11 +1690,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+    <row r="13" spans="2:9" ht="84.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="7" t="s">
         <v>42</v>
       </c>
@@ -1633,10 +1715,10 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="4" t="s">
         <v>44</v>
       </c>
@@ -1667,11 +1749,11 @@
       <c r="G15" s="21"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="2:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+    <row r="16" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
@@ -1684,18 +1766,16 @@
       <c r="G16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H16" s="4"/>
       <c r="I16" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="4" t="s">
         <v>51</v>
       </c>
@@ -1709,17 +1789,17 @@
         <v>15</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="18"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="4" t="s">
         <v>53</v>
       </c>
@@ -1731,17 +1811,17 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+    <row r="19" spans="2:9" ht="129" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="24"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="4" t="s">
         <v>56</v>
       </c>
@@ -1753,17 +1833,17 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I19" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="4" t="s">
         <v>52</v>
       </c>
@@ -1777,17 +1857,17 @@
         <v>18</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="23"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="6" t="s">
         <v>63</v>
       </c>
@@ -1801,7 +1881,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>77</v>
@@ -1814,6 +1894,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -1823,17 +1912,9 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>